<commit_message>
Added work with current model. I estimated that only the higher values will affect the process. As a result, and I calculated an (arbitrary metric to calculate the effect between years.
This was arbitrary and the next idea is to create a function that returns the percentile for each class per year, and estimate the shift of the 10%  (or other percentile for each year), for each of the classes and then calculate the expected 10% value for each distribution and its shift (assuming high correlation here)
</commit_message>
<xml_diff>
--- a/data/baseis.xlsx
+++ b/data/baseis.xlsx
@@ -8,24 +8,39 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_sandbox\misc\dear_niece\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB87E3CE-F3EF-43CB-A574-5312B42A270F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B7E8406-B388-442D-9E88-14F6B1D80C5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Φύλλο1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
+    <sheet name="data-baseis" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <pivotCaches>
+    <pivotCache cacheId="4" r:id="rId3"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="14">
   <si>
     <t>EKPA</t>
   </si>
@@ -55,6 +70,18 @@
   </si>
   <si>
     <t>year</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>Column Labels</t>
+  </si>
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>Sum of entry</t>
   </si>
 </sst>
 </file>
@@ -97,9 +124,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -115,6 +147,274 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Nikos Papadakis" refreshedDate="45834.864488194442" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="21" xr:uid="{C2879FB6-0B38-4253-9710-65D44A88340B}">
+  <cacheSource type="worksheet">
+    <worksheetSource name="Table1"/>
+  </cacheSource>
+  <cacheFields count="4">
+    <cacheField name="id" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="21"/>
+    </cacheField>
+    <cacheField name="School" numFmtId="0">
+      <sharedItems count="7">
+        <s v="EKPA"/>
+        <s v="AUTH"/>
+        <s v="patras"/>
+        <s v="ioannina"/>
+        <s v="Thessaly"/>
+        <s v="Hera"/>
+        <s v="thrace"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="entry" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="17975" maxValue="19000"/>
+    </cacheField>
+    <cacheField name="year" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2022" maxValue="2024" count="3">
+        <n v="2022"/>
+        <n v="2023"/>
+        <n v="2024"/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="21">
+  <r>
+    <n v="1"/>
+    <x v="0"/>
+    <n v="18800"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="2"/>
+    <x v="1"/>
+    <n v="18550"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="3"/>
+    <x v="2"/>
+    <n v="18505"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <x v="3"/>
+    <n v="18275"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="5"/>
+    <x v="4"/>
+    <n v="18200"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="6"/>
+    <x v="5"/>
+    <n v="18150"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="7"/>
+    <x v="6"/>
+    <n v="18075"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="8"/>
+    <x v="0"/>
+    <n v="19000"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="9"/>
+    <x v="1"/>
+    <n v="18800"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="10"/>
+    <x v="2"/>
+    <n v="18735"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="11"/>
+    <x v="3"/>
+    <n v="18475"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="12"/>
+    <x v="4"/>
+    <n v="18450"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="13"/>
+    <x v="5"/>
+    <n v="18400"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="14"/>
+    <x v="6"/>
+    <n v="18300"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="15"/>
+    <x v="0"/>
+    <n v="18775"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="16"/>
+    <x v="1"/>
+    <n v="18550"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="17"/>
+    <x v="2"/>
+    <n v="18460"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="18"/>
+    <x v="3"/>
+    <n v="18200"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="19"/>
+    <x v="4"/>
+    <n v="18125"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="20"/>
+    <x v="5"/>
+    <n v="18050"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="21"/>
+    <x v="6"/>
+    <n v="17975"/>
+    <x v="2"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{AF825A61-DA57-45BF-8718-EC13AA14B0A6}" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:D11" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="4">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="8">
+        <item x="1"/>
+        <item x="0"/>
+        <item x="5"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="4"/>
+        <item x="6"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="7">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="3"/>
+  </colFields>
+  <colItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of entry" fld="2" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{530C6195-CBE8-4B5B-8677-645D6924655F}" name="Table1" displayName="Table1" ref="A1:D22" totalsRowShown="0">
+  <autoFilter ref="A1:D22" xr:uid="{530C6195-CBE8-4B5B-8677-645D6924655F}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D22">
+    <sortCondition ref="A1:A22"/>
+  </sortState>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{15D7C20A-B252-4A5A-B397-EEF02379A94B}" name="id"/>
+    <tableColumn id="2" xr3:uid="{AED7317F-F471-426A-BD0E-C2D1C4DD4F54}" name="School"/>
+    <tableColumn id="3" xr3:uid="{636DEB82-15F6-4A9B-9100-4BE25AE8BF0B}" name="entry"/>
+    <tableColumn id="4" xr3:uid="{BAA92E89-98C5-4B9B-A96C-676A579DDC70}" name="year"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -379,181 +679,468 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:D15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11F60569-4855-422F-A4E8-A70AE52C2FC3}">
+  <dimension ref="A3:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9:D15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.77734375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="1">
-        <v>18775</v>
-      </c>
-      <c r="D2">
-        <v>2024</v>
-      </c>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>18550</v>
-      </c>
-      <c r="D3">
-        <v>2024</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B4" t="s">
-        <v>2</v>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4">
+        <v>2022</v>
       </c>
       <c r="C4">
-        <v>18460</v>
+        <v>2023</v>
       </c>
       <c r="D4">
         <v>2024</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B5" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="4">
+        <v>18550</v>
+      </c>
+      <c r="C5" s="4">
+        <v>18800</v>
+      </c>
+      <c r="D5" s="4">
+        <v>18550</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="4">
+        <v>18800</v>
+      </c>
+      <c r="C6" s="4">
+        <v>19000</v>
+      </c>
+      <c r="D6" s="4">
+        <v>18775</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="4">
+        <v>18150</v>
+      </c>
+      <c r="C7" s="4">
+        <v>18400</v>
+      </c>
+      <c r="D7" s="4">
+        <v>18050</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C5">
+      <c r="B8" s="4">
+        <v>18275</v>
+      </c>
+      <c r="C8" s="4">
+        <v>18475</v>
+      </c>
+      <c r="D8" s="4">
         <v>18200</v>
       </c>
-      <c r="D5">
-        <v>2024</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B6" t="s">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="4">
+        <v>18505</v>
+      </c>
+      <c r="C9" s="4">
+        <v>18735</v>
+      </c>
+      <c r="D9" s="4">
+        <v>18460</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C6">
+      <c r="B10" s="4">
+        <v>18200</v>
+      </c>
+      <c r="C10" s="4">
+        <v>18450</v>
+      </c>
+      <c r="D10" s="4">
         <v>18125</v>
       </c>
-      <c r="D6">
-        <v>2024</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7">
-        <v>18050</v>
-      </c>
-      <c r="D7">
-        <v>2024</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B8" t="s">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C8">
+      <c r="B11" s="4">
+        <v>18075</v>
+      </c>
+      <c r="C11" s="4">
+        <v>18300</v>
+      </c>
+      <c r="D11" s="4">
         <v>17975</v>
-      </c>
-      <c r="D8">
-        <v>2024</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B9" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9" s="1">
-        <v>19000</v>
-      </c>
-      <c r="D9">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10">
-        <v>18800</v>
-      </c>
-      <c r="D10">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11">
-        <v>18735</v>
-      </c>
-      <c r="D11">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B12" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12">
-        <v>18475</v>
-      </c>
-      <c r="D12">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B13" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13">
-        <v>18450</v>
-      </c>
-      <c r="D13">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B14" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14">
-        <v>18400</v>
-      </c>
-      <c r="D14">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15">
-        <v>18300</v>
-      </c>
-      <c r="D15">
-        <v>2023</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>18800</v>
+      </c>
+      <c r="D2">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>18550</v>
+      </c>
+      <c r="D3">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>18505</v>
+      </c>
+      <c r="D4">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>18275</v>
+      </c>
+      <c r="D5">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>18200</v>
+      </c>
+      <c r="D6">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>18150</v>
+      </c>
+      <c r="D7">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <v>18075</v>
+      </c>
+      <c r="D8">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1">
+        <v>19000</v>
+      </c>
+      <c r="D9">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>18800</v>
+      </c>
+      <c r="D10">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>18735</v>
+      </c>
+      <c r="D11">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12">
+        <v>18475</v>
+      </c>
+      <c r="D12">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13">
+        <v>18450</v>
+      </c>
+      <c r="D13">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14">
+        <v>18400</v>
+      </c>
+      <c r="D14">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15">
+        <v>18300</v>
+      </c>
+      <c r="D15">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" s="1">
+        <v>18775</v>
+      </c>
+      <c r="D16">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>18550</v>
+      </c>
+      <c r="D17">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18">
+        <v>18460</v>
+      </c>
+      <c r="D18">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19">
+        <v>18200</v>
+      </c>
+      <c r="D19">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20">
+        <v>18125</v>
+      </c>
+      <c r="D20">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21">
+        <v>18050</v>
+      </c>
+      <c r="D21">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22">
+        <v>17975</v>
+      </c>
+      <c r="D22">
+        <v>2024</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>